<commit_message>
Nuevo archivo de prueba
</commit_message>
<xml_diff>
--- a/Lecciones_test.xlsx
+++ b/Lecciones_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avalbuena\Pictures\Biometrico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbenavides\Desktop\Jupyter\postmortem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28A7A712-B58D-42ED-A9A2-A3625124AAAF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6027E343-6140-41F2-BE4E-E9ED6A2D1936}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{B551BE88-0C10-4456-B249-51B6166F33BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" xr2:uid="{B551BE88-0C10-4456-B249-51B6166F33BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>PROYECTO</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>LECCIONES APRENDIDAS</t>
-  </si>
-  <si>
-    <t>Davi Cargue</t>
   </si>
   <si>
     <t>SWEBOK</t>
@@ -151,21 +148,44 @@
     <t>TRANSFERENCIA DE
  CONOCIIENTO</t>
   </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>The number of use cases of the project was around 100, and yet, for the project life cycle only three increments were defined. The increments of a project should not be greater than one month of development, this allows to execute complete cycles and consequently, to detect problems early</t>
+  </si>
+  <si>
+    <t>The project was assigned two seeds to execute the shadow plan.
+This scheme worked because it was possible to train analysts with technical knowledge and in turn, business transfer was achieved.
+Maintaining knowledge within the organization gives us the opportunity to maintain the trust of our customers, allows us to react to any inconvenience that may arise with the staff.</t>
+  </si>
+  <si>
+    <t>On several occasions in the project, work spaces between Ivan Gonzales, Oscar Arellano and Rodrigo Marrugo could be covered. Having more than one person assigned to the project allows simultaneous requirements to be met at times and that the absence of people does not impact continuity of attention.</t>
+  </si>
+  <si>
+    <t>CO_364 TITULARIZADORA 2015</t>
+  </si>
+  <si>
+    <t>Al generar los paquetes de producción no se revisaban correctamente las configuraciones del ambiente y certificados por tal razón se enviaban con la configuración de pruebas y al tratar de subir estas al servicio en la nube presentaba error, razón por la cual el cliente se quejaba en la atención prestada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antes de generar un paquete a pruebas o producción se deben verificar los valores de las llaves dentro del portal de Azure, además de esto revisar los certificados.
+Se debe revisar los archivos web.config y los cloud.ccproj en los tag que dicen pruebas y/o producción. </t>
+  </si>
+  <si>
+    <t>CALIDAD</t>
+  </si>
+  <si>
+    <t>When generating the production packages, the environment settings were not correctly reviewed and certificates for that reason were sent with the test configuration and when trying to upload them to the cloud service it presented an error, which is why the customer complained in the attention given. Before generating a test or production package, the values of the keys must be verified within the Azure portal, in addition to this review the certificates.
+The web.config and cloud.ccproj files should be checked in the tags that say tests and / or production.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -193,111 +213,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -311,34 +234,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DBBC47B4-E347-4AF1-BC3E-9B8F90F18EBB}" name="Table3" displayName="Table3" ref="A1:R4" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R4" xr:uid="{158BA032-AE7E-4283-8BAA-9C90714F7D6F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DBBC47B4-E347-4AF1-BC3E-9B8F90F18EBB}" name="Table3" displayName="Table3" ref="A1:R4" totalsRowShown="0">
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{D2CF9E7A-674A-48F4-B8DF-0DF32EF77C08}" name="PROYECTO" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{6A6B8912-1E01-4241-A97C-0C14A31BD316}" name="TIPO PROYECTO" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{059E300B-A72D-40EF-941F-13017FAC4E6E}" name="CLIENTE" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{7F813C27-34D0-4E7E-99E3-8C88FCCC35D9}" name="FECHA DE INICIO" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{8E2F4CB0-9010-4373-AE1D-ADD2D26A6DF6}" name="FECHA FINAL" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{B02CBB9E-7F14-4CDE-98D8-2CF20BF023A6}" name="CONTEXTO" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{8E58D02A-C36A-4DEB-BFD0-9484101BB78B}" name="LECCIONES APRENDIDAS" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{0263E832-0FF8-421B-A9BC-FF17B2A757F3}" name="Davi Cargue" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{071F5E4F-DF99-4343-B8D8-366117CA5432}" name="SWEBOK" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{2BD58A3C-C742-4E4F-8083-49DAB7032249}" name="Practices" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{51C6DD75-F016-4FD3-B358-572892EA3319}" name="Paradigma" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{B14FE8FC-8134-4642-8D4F-BEF85F5312AA}" name="Tecnologia" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{2AF6FCB5-35F0-49E6-8425-45745A7FD955}" name="Equipo trabajo" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{7C4C8DB0-8473-48C7-A2AB-4AAD6ADE8E7B}" name="Aporte" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{FBAD8AB9-B72C-4449-8BAC-B02E9768D80F}" name="IMPACTO" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{E7641CEB-B4B0-4464-B5B2-1C77BFCB8B4A}" name="FASE" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{E1A050E2-84D1-4E3A-A447-52AD8A013539}" name="DURACION" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{BB43FAA5-72BF-4357-9B3C-B1158EF7346A}" name="Selección" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D2CF9E7A-674A-48F4-B8DF-0DF32EF77C08}" name="PROYECTO"/>
+    <tableColumn id="2" xr3:uid="{6A6B8912-1E01-4241-A97C-0C14A31BD316}" name="TIPO PROYECTO"/>
+    <tableColumn id="3" xr3:uid="{059E300B-A72D-40EF-941F-13017FAC4E6E}" name="CLIENTE"/>
+    <tableColumn id="4" xr3:uid="{7F813C27-34D0-4E7E-99E3-8C88FCCC35D9}" name="FECHA DE INICIO"/>
+    <tableColumn id="5" xr3:uid="{8E2F4CB0-9010-4373-AE1D-ADD2D26A6DF6}" name="FECHA FINAL"/>
+    <tableColumn id="6" xr3:uid="{B02CBB9E-7F14-4CDE-98D8-2CF20BF023A6}" name="CONTEXTO"/>
+    <tableColumn id="7" xr3:uid="{8E58D02A-C36A-4DEB-BFD0-9484101BB78B}" name="LECCIONES APRENDIDAS"/>
+    <tableColumn id="8" xr3:uid="{0263E832-0FF8-421B-A9BC-FF17B2A757F3}" name="google"/>
+    <tableColumn id="9" xr3:uid="{071F5E4F-DF99-4343-B8D8-366117CA5432}" name="SWEBOK"/>
+    <tableColumn id="10" xr3:uid="{2BD58A3C-C742-4E4F-8083-49DAB7032249}" name="Practices"/>
+    <tableColumn id="11" xr3:uid="{51C6DD75-F016-4FD3-B358-572892EA3319}" name="Paradigma"/>
+    <tableColumn id="12" xr3:uid="{B14FE8FC-8134-4642-8D4F-BEF85F5312AA}" name="Tecnologia"/>
+    <tableColumn id="13" xr3:uid="{2AF6FCB5-35F0-49E6-8425-45745A7FD955}" name="Equipo trabajo"/>
+    <tableColumn id="14" xr3:uid="{7C4C8DB0-8473-48C7-A2AB-4AAD6ADE8E7B}" name="Aporte"/>
+    <tableColumn id="15" xr3:uid="{FBAD8AB9-B72C-4449-8BAC-B02E9768D80F}" name="IMPACTO"/>
+    <tableColumn id="16" xr3:uid="{E7641CEB-B4B0-4464-B5B2-1C77BFCB8B4A}" name="FASE"/>
+    <tableColumn id="17" xr3:uid="{E1A050E2-84D1-4E3A-A447-52AD8A013539}" name="DURACION"/>
+    <tableColumn id="18" xr3:uid="{BB43FAA5-72BF-4357-9B3C-B1158EF7346A}" name="Selección"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -634,191 +556,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319ABDF7-961D-4208-9C61-F76C485A53BB}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="26.42578125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>40961</v>
+      </c>
+      <c r="E2">
+        <v>42229</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2">
+        <v>26222</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4">
-        <v>40961</v>
-      </c>
-      <c r="E2" s="4">
-        <v>42229</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>41835</v>
+      </c>
+      <c r="E3">
+        <v>42311</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3">
+        <v>4987</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>41656</v>
+      </c>
+      <c r="E4">
+        <v>42020</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>42020</v>
+      </c>
+      <c r="E5">
+        <v>42384</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>26222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="3">
-        <v>41835</v>
-      </c>
-      <c r="E3" s="3">
-        <v>42311</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>4987</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="3">
-        <v>41656</v>
-      </c>
-      <c r="E4" s="3">
-        <v>42020</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>2384</v>
+      <c r="P5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5">
+        <v>2027</v>
       </c>
     </row>
   </sheetData>
@@ -831,6 +796,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010006E447E30A1A0C49AF4EC383DE9FF179" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="62063e9950563dedda84c9619c36b0e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8ee99894-d9f1-4b10-bda2-8a07ee0fef8d" xmlns:ns3="7df113a5-70cc-49a4-b8e3-26beca47e62b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb7f6d075e80125099d7e0958b1dc745" ns2:_="" ns3:_="">
     <xsd:import namespace="8ee99894-d9f1-4b10-bda2-8a07ee0fef8d"/>
@@ -1047,7 +1018,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1056,20 +1027,38 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5014F8D-F333-4B44-B294-330268C1790C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6766493E-07E8-4B88-BAE8-44F85BB5C580}"/>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6766493E-07E8-4B88-BAE8-44F85BB5C580}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8ee99894-d9f1-4b10-bda2-8a07ee0fef8d"/>
+    <ds:schemaRef ds:uri="7df113a5-70cc-49a4-b8e3-26beca47e62b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38A1816F-82D8-42F4-A841-306BCEC8BB36}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5014F8D-F333-4B44-B294-330268C1790C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38A1816F-82D8-42F4-A841-306BCEC8BB36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
correccion en leccion 4
</commit_message>
<xml_diff>
--- a/Lecciones_test.xlsx
+++ b/Lecciones_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbenavides\Desktop\Jupyter\postmortem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6027E343-6140-41F2-BE4E-E9ED6A2D1936}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953D6A64-359D-4E16-82F4-BEC9AEF849A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" xr2:uid="{B551BE88-0C10-4456-B249-51B6166F33BD}"/>
   </bookViews>
@@ -176,8 +176,7 @@
     <t>CALIDAD</t>
   </si>
   <si>
-    <t>When generating the production packages, the environment settings were not correctly reviewed and certificates for that reason were sent with the test configuration and when trying to upload them to the cloud service it presented an error, which is why the customer complained in the attention given. Before generating a test or production package, the values of the keys must be verified within the Azure portal, in addition to this review the certificates.
-The web.config and cloud.ccproj files should be checked in the tags that say tests and / or production.</t>
+    <t>When generating the production packages, the environment settings were not correctly reviewed and certificates for that reason were sent with the test configuration and when trying to upload them to the cloud service it presented an error, which is why the customer complained in the attention given. Before generating a test or production package, the values of the keys must be verified within the Azure portal, in addition to this review the certificates. The web.config and cloud.ccproj files should be checked in the tags that say tests and / or production.</t>
   </si>
 </sst>
 </file>
@@ -559,7 +558,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,9 +795,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1019,19 +1021,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5014F8D-F333-4B44-B294-330268C1790C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38A1816F-82D8-42F4-A841-306BCEC8BB36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1056,9 +1054,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38A1816F-82D8-42F4-A841-306BCEC8BB36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5014F8D-F333-4B44-B294-330268C1790C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>